<commit_message>
apiAuto_v10, validate the data in the database using sql
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase_v10.xlsx
+++ b/src/test/resources/TestCase_v10.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaa./Documents/project/apiAuto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ECA136-9935-1E43-A1C9-E720D4A918D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{06011F19-BD2E-9A4E-B536-F012D496F217}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="1120" windowWidth="27440" windowHeight="16540" xr2:uid="{03CFF585-8EAA-974E-B709-D7D4176395E7}"/>
+    <workbookView activeTab="1" windowHeight="16540" windowWidth="27440" xWindow="1360" xr2:uid="{03CFF585-8EAA-974E-B709-D7D4176395E7}" yWindow="1120"/>
   </bookViews>
   <sheets>
-    <sheet name="ApiInfoSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="CaseInfoSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="ApiInfoSheet" r:id="rId1" sheetId="1"/>
+    <sheet name="CaseInfoSheet" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
   <si>
     <t>CaseId(用例编号)</t>
   </si>
@@ -308,13 +308,29 @@
   </si>
   <si>
     <t>http://47.107.166.132:8080/futureloan/mvc/api/financelog/getFinanceLogList</t>
+  </si>
+  <si>
+    <t>[{“no”:”1”,”sql”:”select count(*) as totalNum from member where mobilephone=’13517315120’”}]</t>
+  </si>
+  <si>
+    <t>[{"no":"1","sql":"select leaveamount from member where mobilephone='13517315120'"}, {"no":"2","sql":"select count(*) as totalNum from financelog where IncomeMemberId = (select id from member where mobilephone='13517315120'"}]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>{"status":0,"code":"20116","data":null,"msg":"输入金额的金额小数不能超过两位"}</t>
+  </si>
+  <si>
+    <t>{"status":1,"code":"10001","data":{"id":360,"regname":"小蜜蜂","pwd":"E10ADC3949BA59ABBE56E057F20F883E","mobilephone":"18813989007","leaveamount":"100000.00","type":"1","regtime":"2019-10-06 09:54:57.0"},"msg":"充值成功"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,8 +342,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -348,37 +370,41 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -395,10 +421,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -433,7 +459,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -485,7 +511,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -596,21 +622,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -627,7 +653,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -679,26 +705,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72445A8-64EA-6546-9F38-72C432B7D5E6}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72445A8-64EA-6546-9F38-72C432B7D5E6}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="80" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="22.33203125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="24.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="80.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -898,33 +924,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADF37B3-C487-1545-B431-E4A62F8DA59B}">
-  <dimension ref="A1:J21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADF37B3-C487-1545-B431-E4A62F8DA59B}">
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="77.83203125" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" customWidth="1"/>
-    <col min="8" max="8" width="52.1640625" customWidth="1"/>
-    <col min="9" max="9" width="40.33203125" customWidth="1"/>
-    <col min="10" max="10" width="47.5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.83203125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="19.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="21.83203125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="77.83203125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="36.6640625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="204.33203125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="52.1640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="40.33203125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="47.5" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" customHeight="1" ht="18" r="1" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,7 +982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" customHeight="1" ht="12" r="2" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -972,8 +998,11 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -989,9 +1018,11 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row customFormat="1" r="4" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1007,9 +1038,11 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row customFormat="1" r="5" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1025,9 +1058,11 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="50" r="6" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1043,8 +1078,17 @@
       <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1060,8 +1104,11 @@
       <c r="E7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row customFormat="1" r="8" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1077,8 +1124,11 @@
       <c r="E8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="9" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1094,8 +1144,11 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row customFormat="1" r="10" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1111,8 +1164,11 @@
       <c r="E10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1128,8 +1184,11 @@
       <c r="E11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row customFormat="1" r="12" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1145,8 +1204,11 @@
       <c r="E12" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row customFormat="1" r="13" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1162,8 +1224,11 @@
       <c r="E13" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row customFormat="1" r="14" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1179,8 +1244,11 @@
       <c r="E14" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row customFormat="1" r="15" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1196,8 +1264,11 @@
       <c r="E15" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row customFormat="1" r="16" s="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1213,8 +1284,11 @@
       <c r="E16" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row customFormat="1" r="17" s="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1230,8 +1304,11 @@
       <c r="E17" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row customFormat="1" r="18" s="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1247,8 +1324,11 @@
       <c r="E18" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row customFormat="1" r="19" s="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1264,8 +1344,11 @@
       <c r="E19" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row customFormat="1" r="20" s="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1281,8 +1364,11 @@
       <c r="E20" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row customFormat="1" r="21" s="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1298,8 +1384,17 @@
       <c r="E21" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>